<commit_message>
test fixed portfolio 1
</commit_message>
<xml_diff>
--- a/.xlsx/current_quarter_classification.xlsx
+++ b/.xlsx/current_quarter_classification.xlsx
@@ -868,7 +868,11 @@
           <t>DV hạ tầng</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr">
         <is>
           <t>penny</t>
@@ -1478,7 +1482,11 @@
           <t>Bất động sản</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H26" t="inlineStr">
         <is>
           <t>small</t>
@@ -1932,7 +1940,11 @@
           <t>Xây dựng</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H37" t="inlineStr">
         <is>
           <t>small</t>
@@ -2176,7 +2188,11 @@
           <t>Bất động sản</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H43" t="inlineStr">
         <is>
           <t>mid</t>
@@ -2988,7 +3004,11 @@
           <t>Chứng khoán</t>
         </is>
       </c>
-      <c r="G63" t="inlineStr"/>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H63" t="inlineStr">
         <is>
           <t>small</t>
@@ -3430,7 +3450,11 @@
           <t>Công ty tài chính</t>
         </is>
       </c>
-      <c r="G74" t="inlineStr"/>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H74" t="inlineStr">
         <is>
           <t>penny</t>
@@ -3468,7 +3492,11 @@
           <t>Bất động sản</t>
         </is>
       </c>
-      <c r="G75" t="inlineStr"/>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H75" t="inlineStr">
         <is>
           <t>small</t>
@@ -3632,7 +3660,11 @@
           <t>DV hạ tầng</t>
         </is>
       </c>
-      <c r="G79" t="inlineStr"/>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H79" t="inlineStr">
         <is>
           <t>small</t>
@@ -3712,7 +3744,11 @@
           <t>DV hạ tầng</t>
         </is>
       </c>
-      <c r="G81" t="inlineStr"/>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H81" t="inlineStr">
         <is>
           <t>small</t>
@@ -3956,7 +3992,11 @@
           <t>Xây dựng</t>
         </is>
       </c>
-      <c r="G87" t="inlineStr"/>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H87" t="inlineStr">
         <is>
           <t>small</t>
@@ -4276,7 +4316,11 @@
           <t>Y tế</t>
         </is>
       </c>
-      <c r="G95" t="inlineStr"/>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H95" t="inlineStr">
         <is>
           <t>penny</t>
@@ -4356,7 +4400,11 @@
           <t>Thực phẩm</t>
         </is>
       </c>
-      <c r="G97" t="inlineStr"/>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H97" t="inlineStr">
         <is>
           <t>small</t>
@@ -4714,7 +4762,11 @@
           <t>Y tế</t>
         </is>
       </c>
-      <c r="G106" t="inlineStr"/>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H106" t="inlineStr">
         <is>
           <t>mid</t>
@@ -5430,7 +5482,11 @@
           <t>Xây dựng</t>
         </is>
       </c>
-      <c r="G124" t="inlineStr"/>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H124" t="inlineStr">
         <is>
           <t>penny</t>
@@ -5762,7 +5818,11 @@
           <t>Xây dựng</t>
         </is>
       </c>
-      <c r="G132" t="inlineStr"/>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H132" t="inlineStr">
         <is>
           <t>penny</t>
@@ -5842,7 +5902,11 @@
           <t>Công nghiệp</t>
         </is>
       </c>
-      <c r="G134" t="inlineStr"/>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H134" t="inlineStr">
         <is>
           <t>penny</t>
@@ -6204,7 +6268,11 @@
           <t>Bán lẻ</t>
         </is>
       </c>
-      <c r="G143" t="inlineStr"/>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H143" t="inlineStr">
         <is>
           <t>small</t>
@@ -6242,7 +6310,11 @@
           <t>Hoá chất</t>
         </is>
       </c>
-      <c r="G144" t="inlineStr"/>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H144" t="inlineStr">
         <is>
           <t>small</t>
@@ -6524,7 +6596,11 @@
           <t>DV hạ tầng</t>
         </is>
       </c>
-      <c r="G151" t="inlineStr"/>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H151" t="inlineStr">
         <is>
           <t>small</t>
@@ -6688,7 +6764,11 @@
           <t>Vận tải</t>
         </is>
       </c>
-      <c r="G155" t="inlineStr"/>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H155" t="inlineStr">
         <is>
           <t>small</t>
@@ -6768,7 +6848,11 @@
           <t>Y tế</t>
         </is>
       </c>
-      <c r="G157" t="inlineStr"/>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H157" t="inlineStr">
         <is>
           <t>small</t>
@@ -6928,7 +7012,11 @@
           <t>Xây dựng</t>
         </is>
       </c>
-      <c r="G161" t="inlineStr"/>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H161" t="inlineStr">
         <is>
           <t>small</t>
@@ -7286,7 +7374,11 @@
           <t>Bảo hiểm</t>
         </is>
       </c>
-      <c r="G170" t="inlineStr"/>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H170" t="inlineStr">
         <is>
           <t>small</t>
@@ -7324,7 +7416,11 @@
           <t>Khoáng sản</t>
         </is>
       </c>
-      <c r="G171" t="inlineStr"/>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H171" t="inlineStr">
         <is>
           <t>small</t>
@@ -7488,7 +7584,11 @@
           <t>Thực phẩm</t>
         </is>
       </c>
-      <c r="G175" t="inlineStr"/>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H175" t="inlineStr">
         <is>
           <t>small</t>
@@ -7804,7 +7904,11 @@
           <t>Công nghệ</t>
         </is>
       </c>
-      <c r="G183" t="inlineStr"/>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H183" t="inlineStr">
         <is>
           <t>penny</t>
@@ -8002,7 +8106,11 @@
           <t>Y tế</t>
         </is>
       </c>
-      <c r="G188" t="inlineStr"/>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H188" t="inlineStr">
         <is>
           <t>penny</t>
@@ -8246,7 +8354,11 @@
           <t>Thép</t>
         </is>
       </c>
-      <c r="G194" t="inlineStr"/>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H194" t="inlineStr">
         <is>
           <t>small</t>
@@ -8558,7 +8670,11 @@
           <t>Y tế</t>
         </is>
       </c>
-      <c r="G202" t="inlineStr"/>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H202" t="inlineStr">
         <is>
           <t>small</t>
@@ -9008,7 +9124,11 @@
           <t>DV hạ tầng</t>
         </is>
       </c>
-      <c r="G213" t="inlineStr"/>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H213" t="inlineStr">
         <is>
           <t>penny</t>
@@ -9888,7 +10008,11 @@
           <t>Hoá chất</t>
         </is>
       </c>
-      <c r="G235" t="inlineStr"/>
+      <c r="G235" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H235" t="inlineStr">
         <is>
           <t>small</t>
@@ -10052,7 +10176,11 @@
           <t>Bất động sản</t>
         </is>
       </c>
-      <c r="G239" t="inlineStr"/>
+      <c r="G239" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H239" t="inlineStr">
         <is>
           <t>small</t>
@@ -10212,7 +10340,11 @@
           <t>Khoáng sản</t>
         </is>
       </c>
-      <c r="G243" t="inlineStr"/>
+      <c r="G243" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H243" t="inlineStr">
         <is>
           <t>penny</t>
@@ -10330,7 +10462,11 @@
           <t>Ngân hàng</t>
         </is>
       </c>
-      <c r="G246" t="inlineStr"/>
+      <c r="G246" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H246" t="inlineStr">
         <is>
           <t>mid</t>
@@ -10528,7 +10664,11 @@
           <t>Y tế</t>
         </is>
       </c>
-      <c r="G251" t="inlineStr"/>
+      <c r="G251" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H251" t="inlineStr">
         <is>
           <t>mid</t>
@@ -11252,7 +11392,11 @@
           <t>Hoá chất</t>
         </is>
       </c>
-      <c r="G269" t="inlineStr"/>
+      <c r="G269" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H269" t="inlineStr">
         <is>
           <t>penny</t>
@@ -11412,7 +11556,11 @@
           <t>Xây dựng</t>
         </is>
       </c>
-      <c r="G273" t="inlineStr"/>
+      <c r="G273" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H273" t="inlineStr">
         <is>
           <t>penny</t>
@@ -11774,7 +11922,11 @@
           <t>Ngân hàng</t>
         </is>
       </c>
-      <c r="G282" t="inlineStr"/>
+      <c r="G282" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H282" t="inlineStr">
         <is>
           <t>small</t>
@@ -12018,7 +12170,11 @@
           <t>Ngân hàng</t>
         </is>
       </c>
-      <c r="G288" t="inlineStr"/>
+      <c r="G288" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H288" t="inlineStr">
         <is>
           <t>mid</t>
@@ -12098,7 +12254,11 @@
           <t>Chứng khoán</t>
         </is>
       </c>
-      <c r="G290" t="inlineStr"/>
+      <c r="G290" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H290" t="inlineStr">
         <is>
           <t>small</t>
@@ -12178,7 +12338,11 @@
           <t>Xây dựng</t>
         </is>
       </c>
-      <c r="G292" t="inlineStr"/>
+      <c r="G292" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H292" t="inlineStr">
         <is>
           <t>penny</t>
@@ -12384,7 +12548,11 @@
           <t>Vận tải</t>
         </is>
       </c>
-      <c r="G297" t="inlineStr"/>
+      <c r="G297" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H297" t="inlineStr">
         <is>
           <t>small</t>
@@ -12422,7 +12590,11 @@
           <t>Thực phẩm</t>
         </is>
       </c>
-      <c r="G298" t="inlineStr"/>
+      <c r="G298" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H298" t="inlineStr">
         <is>
           <t>penny</t>
@@ -12864,7 +13036,11 @@
           <t>DV hạ tầng</t>
         </is>
       </c>
-      <c r="G309" t="inlineStr"/>
+      <c r="G309" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H309" t="inlineStr">
         <is>
           <t>small</t>
@@ -12902,7 +13078,11 @@
           <t>Thực phẩm</t>
         </is>
       </c>
-      <c r="G310" t="inlineStr"/>
+      <c r="G310" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H310" t="inlineStr">
         <is>
           <t>penny</t>
@@ -13332,7 +13512,11 @@
           <t>Hoá chất</t>
         </is>
       </c>
-      <c r="G321" t="inlineStr"/>
+      <c r="G321" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H321" t="inlineStr">
         <is>
           <t>small</t>
@@ -13614,7 +13798,11 @@
           <t>Khoáng sản</t>
         </is>
       </c>
-      <c r="G328" t="inlineStr"/>
+      <c r="G328" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H328" t="inlineStr">
         <is>
           <t>small</t>

</xml_diff>